<commit_message>
OW-972, updated the tests
</commit_message>
<xml_diff>
--- a/test/availAsset.xlsx
+++ b/test/availAsset.xlsx
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="B46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16:O58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,10 +686,10 @@
         <v>16</v>
       </c>
       <c r="J2">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K2">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -701,7 +701,7 @@
         <v>0.08</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -739,10 +739,10 @@
         <v>16</v>
       </c>
       <c r="J3">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K3">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -754,7 +754,7 @@
         <v>0.08</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -792,10 +792,10 @@
         <v>16</v>
       </c>
       <c r="J4">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K4">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -807,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -845,10 +845,10 @@
         <v>16</v>
       </c>
       <c r="J5">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K5">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -860,7 +860,7 @@
         <v>0.08</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -898,10 +898,10 @@
         <v>16</v>
       </c>
       <c r="J6">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K6">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -913,7 +913,7 @@
         <v>0.08</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -951,10 +951,10 @@
         <v>16</v>
       </c>
       <c r="J7">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K7">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -966,7 +966,7 @@
         <v>0.08</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1004,10 +1004,10 @@
         <v>16</v>
       </c>
       <c r="J8">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K8">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1019,7 +1019,7 @@
         <v>0.08</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1057,10 +1057,10 @@
         <v>16</v>
       </c>
       <c r="J9">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K9">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1072,7 +1072,7 @@
         <v>0.08</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1110,10 +1110,10 @@
         <v>16</v>
       </c>
       <c r="J10">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K10">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1125,7 +1125,7 @@
         <v>0.08</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1163,10 +1163,10 @@
         <v>16</v>
       </c>
       <c r="J11">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K11">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1178,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1216,10 +1216,10 @@
         <v>16</v>
       </c>
       <c r="J12">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K12">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1231,7 +1231,7 @@
         <v>0.08</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1269,10 +1269,10 @@
         <v>16</v>
       </c>
       <c r="J13">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K13">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1284,7 +1284,7 @@
         <v>0.08</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -1322,10 +1322,10 @@
         <v>16</v>
       </c>
       <c r="J14">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K14">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -1337,7 +1337,7 @@
         <v>0.08</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -1375,10 +1375,10 @@
         <v>16</v>
       </c>
       <c r="J15">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K15">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1390,7 +1390,7 @@
         <v>0.08</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -1428,10 +1428,10 @@
         <v>16</v>
       </c>
       <c r="J16" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K16" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L16" s="2">
         <v>0</v>
@@ -1442,8 +1442,8 @@
       <c r="N16">
         <v>0.08</v>
       </c>
-      <c r="O16" s="2">
-        <v>2E-3</v>
+      <c r="O16">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P16" s="2">
         <v>0</v>
@@ -1481,10 +1481,10 @@
         <v>16</v>
       </c>
       <c r="J17" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K17" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L17" s="2">
         <v>0</v>
@@ -1495,8 +1495,8 @@
       <c r="N17">
         <v>0.08</v>
       </c>
-      <c r="O17" s="2">
-        <v>2E-3</v>
+      <c r="O17">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P17" s="2">
         <v>0</v>
@@ -1534,10 +1534,10 @@
         <v>16</v>
       </c>
       <c r="J18" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K18" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L18" s="2">
         <v>0</v>
@@ -1548,8 +1548,8 @@
       <c r="N18">
         <v>0.08</v>
       </c>
-      <c r="O18" s="2">
-        <v>2E-3</v>
+      <c r="O18">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P18" s="2">
         <v>0</v>
@@ -1587,10 +1587,10 @@
         <v>16</v>
       </c>
       <c r="J19" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K19" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L19" s="2">
         <v>0</v>
@@ -1601,8 +1601,8 @@
       <c r="N19">
         <v>0.08</v>
       </c>
-      <c r="O19" s="2">
-        <v>2E-3</v>
+      <c r="O19">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P19" s="2">
         <v>0</v>
@@ -1640,10 +1640,10 @@
         <v>16</v>
       </c>
       <c r="J20" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K20" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L20" s="2">
         <v>0</v>
@@ -1654,8 +1654,8 @@
       <c r="N20">
         <v>0.08</v>
       </c>
-      <c r="O20" s="2">
-        <v>2E-3</v>
+      <c r="O20">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P20" s="2">
         <v>0</v>
@@ -1693,10 +1693,10 @@
         <v>16</v>
       </c>
       <c r="J21" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K21" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L21" s="2">
         <v>0</v>
@@ -1707,8 +1707,8 @@
       <c r="N21">
         <v>0.08</v>
       </c>
-      <c r="O21" s="2">
-        <v>2E-3</v>
+      <c r="O21">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P21" s="2">
         <v>0</v>
@@ -1746,10 +1746,10 @@
         <v>16</v>
       </c>
       <c r="J22" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K22" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L22" s="2">
         <v>0</v>
@@ -1760,8 +1760,8 @@
       <c r="N22">
         <v>0.08</v>
       </c>
-      <c r="O22" s="2">
-        <v>2E-3</v>
+      <c r="O22">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P22" s="2">
         <v>0</v>
@@ -1799,10 +1799,10 @@
         <v>16</v>
       </c>
       <c r="J23" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K23" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L23" s="2">
         <v>0</v>
@@ -1813,8 +1813,8 @@
       <c r="N23">
         <v>0.08</v>
       </c>
-      <c r="O23" s="2">
-        <v>2E-3</v>
+      <c r="O23">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P23" s="2">
         <v>0</v>
@@ -1852,10 +1852,10 @@
         <v>16</v>
       </c>
       <c r="J24" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K24" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L24" s="2">
         <v>0</v>
@@ -1866,8 +1866,8 @@
       <c r="N24">
         <v>0.08</v>
       </c>
-      <c r="O24" s="2">
-        <v>2E-3</v>
+      <c r="O24">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P24" s="2">
         <v>0</v>
@@ -1905,10 +1905,10 @@
         <v>16</v>
       </c>
       <c r="J25" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K25" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L25" s="2">
         <v>0</v>
@@ -1919,8 +1919,8 @@
       <c r="N25">
         <v>0.08</v>
       </c>
-      <c r="O25" s="2">
-        <v>2E-3</v>
+      <c r="O25">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P25" s="2">
         <v>0</v>
@@ -1958,10 +1958,10 @@
         <v>16</v>
       </c>
       <c r="J26" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K26" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L26" s="2">
         <v>0</v>
@@ -1972,8 +1972,8 @@
       <c r="N26">
         <v>0.08</v>
       </c>
-      <c r="O26" s="2">
-        <v>2E-3</v>
+      <c r="O26">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P26" s="2">
         <v>0</v>
@@ -2011,10 +2011,10 @@
         <v>16</v>
       </c>
       <c r="J27" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K27" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L27" s="2">
         <v>0</v>
@@ -2025,8 +2025,8 @@
       <c r="N27">
         <v>0.08</v>
       </c>
-      <c r="O27" s="2">
-        <v>2E-3</v>
+      <c r="O27">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P27" s="2">
         <v>0</v>
@@ -2064,10 +2064,10 @@
         <v>16</v>
       </c>
       <c r="J28" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K28" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L28" s="2">
         <v>0</v>
@@ -2078,8 +2078,8 @@
       <c r="N28">
         <v>0.08</v>
       </c>
-      <c r="O28" s="2">
-        <v>2E-3</v>
+      <c r="O28">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P28" s="2">
         <v>0</v>
@@ -2117,10 +2117,10 @@
         <v>16</v>
       </c>
       <c r="J29" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K29" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L29" s="2">
         <v>0</v>
@@ -2131,8 +2131,8 @@
       <c r="N29">
         <v>0.08</v>
       </c>
-      <c r="O29" s="2">
-        <v>2E-3</v>
+      <c r="O29">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P29" s="2">
         <v>0</v>
@@ -2170,10 +2170,10 @@
         <v>16</v>
       </c>
       <c r="J30" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K30" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L30" s="2">
         <v>0</v>
@@ -2184,8 +2184,8 @@
       <c r="N30">
         <v>0.08</v>
       </c>
-      <c r="O30" s="2">
-        <v>2E-3</v>
+      <c r="O30">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P30" s="2">
         <v>0</v>
@@ -2223,10 +2223,10 @@
         <v>16</v>
       </c>
       <c r="J31" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K31" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L31" s="2">
         <v>0</v>
@@ -2237,8 +2237,8 @@
       <c r="N31">
         <v>0.08</v>
       </c>
-      <c r="O31" s="2">
-        <v>2E-3</v>
+      <c r="O31">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P31" s="2">
         <v>0</v>
@@ -2276,10 +2276,10 @@
         <v>16</v>
       </c>
       <c r="J32" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K32" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L32" s="2">
         <v>0</v>
@@ -2290,8 +2290,8 @@
       <c r="N32">
         <v>0.08</v>
       </c>
-      <c r="O32" s="2">
-        <v>2E-3</v>
+      <c r="O32">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P32" s="2">
         <v>0</v>
@@ -2329,10 +2329,10 @@
         <v>16</v>
       </c>
       <c r="J33" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K33" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L33" s="2">
         <v>0</v>
@@ -2343,8 +2343,8 @@
       <c r="N33">
         <v>0.08</v>
       </c>
-      <c r="O33" s="2">
-        <v>2E-3</v>
+      <c r="O33">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P33" s="2">
         <v>0</v>
@@ -2382,10 +2382,10 @@
         <v>16</v>
       </c>
       <c r="J34" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K34" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L34" s="2">
         <v>0</v>
@@ -2396,8 +2396,8 @@
       <c r="N34">
         <v>0.08</v>
       </c>
-      <c r="O34" s="2">
-        <v>2E-3</v>
+      <c r="O34">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P34" s="2">
         <v>0</v>
@@ -2435,10 +2435,10 @@
         <v>16</v>
       </c>
       <c r="J35" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K35" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L35" s="2">
         <v>0</v>
@@ -2449,8 +2449,8 @@
       <c r="N35">
         <v>0.08</v>
       </c>
-      <c r="O35" s="2">
-        <v>2E-3</v>
+      <c r="O35">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P35" s="2">
         <v>0</v>
@@ -2488,10 +2488,10 @@
         <v>16</v>
       </c>
       <c r="J36" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K36" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L36" s="2">
         <v>0</v>
@@ -2502,8 +2502,8 @@
       <c r="N36">
         <v>0.08</v>
       </c>
-      <c r="O36" s="2">
-        <v>2E-3</v>
+      <c r="O36">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P36" s="2">
         <v>0</v>
@@ -2541,10 +2541,10 @@
         <v>16</v>
       </c>
       <c r="J37" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K37" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L37" s="2">
         <v>0</v>
@@ -2555,8 +2555,8 @@
       <c r="N37">
         <v>0.08</v>
       </c>
-      <c r="O37" s="2">
-        <v>5.0000000000000001E-3</v>
+      <c r="O37">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P37" s="2">
         <v>0</v>
@@ -2594,10 +2594,10 @@
         <v>16</v>
       </c>
       <c r="J38" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K38" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L38" s="2">
         <v>0</v>
@@ -2608,8 +2608,8 @@
       <c r="N38">
         <v>0.08</v>
       </c>
-      <c r="O38" s="2">
-        <v>5.0000000000000001E-3</v>
+      <c r="O38">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P38" s="2">
         <v>0</v>
@@ -2647,10 +2647,10 @@
         <v>16</v>
       </c>
       <c r="J39" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K39" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L39" s="2">
         <v>0</v>
@@ -2661,8 +2661,8 @@
       <c r="N39">
         <v>0.08</v>
       </c>
-      <c r="O39" s="2">
-        <v>5.0000000000000001E-3</v>
+      <c r="O39">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P39" s="2">
         <v>0</v>
@@ -2700,10 +2700,10 @@
         <v>16</v>
       </c>
       <c r="J40" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K40" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L40" s="2">
         <v>0</v>
@@ -2714,8 +2714,8 @@
       <c r="N40">
         <v>0.08</v>
       </c>
-      <c r="O40" s="2">
-        <v>5.0000000000000001E-3</v>
+      <c r="O40">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P40" s="2">
         <v>0</v>
@@ -2753,10 +2753,10 @@
         <v>16</v>
       </c>
       <c r="J41" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K41" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L41" s="2">
         <v>0</v>
@@ -2767,8 +2767,8 @@
       <c r="N41">
         <v>0.08</v>
       </c>
-      <c r="O41" s="2">
-        <v>5.0000000000000001E-3</v>
+      <c r="O41">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P41" s="2">
         <v>0</v>
@@ -2806,10 +2806,10 @@
         <v>16</v>
       </c>
       <c r="J42" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K42" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L42" s="2">
         <v>0</v>
@@ -2820,8 +2820,8 @@
       <c r="N42">
         <v>0.08</v>
       </c>
-      <c r="O42" s="2">
-        <v>5.0000000000000001E-3</v>
+      <c r="O42">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P42" s="2">
         <v>0</v>
@@ -2859,10 +2859,10 @@
         <v>16</v>
       </c>
       <c r="J43" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K43" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L43" s="2">
         <v>0</v>
@@ -2873,8 +2873,8 @@
       <c r="N43">
         <v>0.08</v>
       </c>
-      <c r="O43" s="2">
-        <v>2E-3</v>
+      <c r="O43">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P43" s="2">
         <v>0</v>
@@ -2912,10 +2912,10 @@
         <v>16</v>
       </c>
       <c r="J44" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K44" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L44" s="2">
         <v>0</v>
@@ -2926,8 +2926,8 @@
       <c r="N44">
         <v>0.08</v>
       </c>
-      <c r="O44" s="2">
-        <v>2E-3</v>
+      <c r="O44">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P44" s="2">
         <v>0</v>
@@ -2965,10 +2965,10 @@
         <v>16</v>
       </c>
       <c r="J45" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K45" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L45" s="2">
         <v>0</v>
@@ -2979,8 +2979,8 @@
       <c r="N45">
         <v>0.08</v>
       </c>
-      <c r="O45" s="2">
-        <v>2E-3</v>
+      <c r="O45">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P45" s="2">
         <v>0</v>
@@ -3018,10 +3018,10 @@
         <v>16</v>
       </c>
       <c r="J46" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K46" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L46" s="2">
         <v>0</v>
@@ -3032,8 +3032,8 @@
       <c r="N46">
         <v>0.08</v>
       </c>
-      <c r="O46" s="2">
-        <v>2E-3</v>
+      <c r="O46">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P46" s="2">
         <v>0</v>
@@ -3071,10 +3071,10 @@
         <v>16</v>
       </c>
       <c r="J47" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K47" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L47" s="2">
         <v>0</v>
@@ -3085,8 +3085,8 @@
       <c r="N47">
         <v>0.08</v>
       </c>
-      <c r="O47" s="2">
-        <v>2E-3</v>
+      <c r="O47">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P47" s="2">
         <v>0</v>
@@ -3124,10 +3124,10 @@
         <v>16</v>
       </c>
       <c r="J48" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K48" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L48" s="2">
         <v>0</v>
@@ -3138,8 +3138,8 @@
       <c r="N48">
         <v>0.08</v>
       </c>
-      <c r="O48" s="2">
-        <v>2E-3</v>
+      <c r="O48">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P48" s="2">
         <v>0</v>
@@ -3177,10 +3177,10 @@
         <v>16</v>
       </c>
       <c r="J49" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K49" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L49" s="2">
         <v>0</v>
@@ -3191,8 +3191,8 @@
       <c r="N49">
         <v>0</v>
       </c>
-      <c r="O49" s="2">
-        <v>2E-3</v>
+      <c r="O49">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P49" s="2">
         <v>0</v>
@@ -3230,10 +3230,10 @@
         <v>16</v>
       </c>
       <c r="J50" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K50" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L50" s="2">
         <v>0</v>
@@ -3244,8 +3244,8 @@
       <c r="N50">
         <v>0</v>
       </c>
-      <c r="O50" s="2">
-        <v>2E-3</v>
+      <c r="O50">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P50" s="2">
         <v>0</v>
@@ -3283,10 +3283,10 @@
         <v>16</v>
       </c>
       <c r="J51" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K51" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L51" s="2">
         <v>0</v>
@@ -3297,8 +3297,8 @@
       <c r="N51">
         <v>0</v>
       </c>
-      <c r="O51" s="2">
-        <v>2E-3</v>
+      <c r="O51">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P51" s="2">
         <v>0</v>
@@ -3336,10 +3336,10 @@
         <v>16</v>
       </c>
       <c r="J52" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K52" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L52" s="2">
         <v>0</v>
@@ -3350,8 +3350,8 @@
       <c r="N52">
         <v>0.08</v>
       </c>
-      <c r="O52" s="2">
-        <v>2E-3</v>
+      <c r="O52">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P52" s="2">
         <v>0</v>
@@ -3389,10 +3389,10 @@
         <v>16</v>
       </c>
       <c r="J53" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K53" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L53" s="2">
         <v>0</v>
@@ -3403,8 +3403,8 @@
       <c r="N53">
         <v>0.08</v>
       </c>
-      <c r="O53" s="2">
-        <v>2E-3</v>
+      <c r="O53">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P53" s="2">
         <v>0</v>
@@ -3442,10 +3442,10 @@
         <v>16</v>
       </c>
       <c r="J54" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K54" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L54" s="2">
         <v>0</v>
@@ -3456,8 +3456,8 @@
       <c r="N54">
         <v>0.08</v>
       </c>
-      <c r="O54" s="2">
-        <v>2E-3</v>
+      <c r="O54">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P54" s="2">
         <v>0</v>
@@ -3495,10 +3495,10 @@
         <v>16</v>
       </c>
       <c r="J55" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K55" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L55" s="2">
         <v>0</v>
@@ -3509,8 +3509,8 @@
       <c r="N55">
         <v>0.08</v>
       </c>
-      <c r="O55" s="2">
-        <v>2E-3</v>
+      <c r="O55">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P55" s="2">
         <v>0</v>
@@ -3548,10 +3548,10 @@
         <v>16</v>
       </c>
       <c r="J56" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K56" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L56" s="2">
         <v>0</v>
@@ -3562,8 +3562,8 @@
       <c r="N56">
         <v>0.08</v>
       </c>
-      <c r="O56" s="2">
-        <v>2E-3</v>
+      <c r="O56">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P56" s="2">
         <v>0</v>
@@ -3601,10 +3601,10 @@
         <v>16</v>
       </c>
       <c r="J57" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K57" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L57" s="2">
         <v>0</v>
@@ -3615,8 +3615,8 @@
       <c r="N57">
         <v>0.08</v>
       </c>
-      <c r="O57" s="2">
-        <v>2E-3</v>
+      <c r="O57">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P57" s="2">
         <v>0</v>
@@ -3654,10 +3654,10 @@
         <v>16</v>
       </c>
       <c r="J58" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K58" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L58" s="2">
         <v>0</v>
@@ -3668,8 +3668,8 @@
       <c r="N58">
         <v>0.08</v>
       </c>
-      <c r="O58" s="2">
-        <v>2E-3</v>
+      <c r="O58">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P58" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Revert "OW-972, updated the tests"
This reverts commit 556ecdda2a0ec00faa94dcd0288e72a6a6892e81.
</commit_message>
<xml_diff>
--- a/test/availAsset.xlsx
+++ b/test/availAsset.xlsx
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16:O58"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,10 +686,10 @@
         <v>16</v>
       </c>
       <c r="J2">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K2">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -701,7 +701,7 @@
         <v>0.08</v>
       </c>
       <c r="O2">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -739,10 +739,10 @@
         <v>16</v>
       </c>
       <c r="J3">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K3">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -754,7 +754,7 @@
         <v>0.08</v>
       </c>
       <c r="O3">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -792,10 +792,10 @@
         <v>16</v>
       </c>
       <c r="J4">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K4">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -807,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -845,10 +845,10 @@
         <v>16</v>
       </c>
       <c r="J5">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K5">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -860,7 +860,7 @@
         <v>0.08</v>
       </c>
       <c r="O5">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -898,10 +898,10 @@
         <v>16</v>
       </c>
       <c r="J6">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K6">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -913,7 +913,7 @@
         <v>0.08</v>
       </c>
       <c r="O6">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -951,10 +951,10 @@
         <v>16</v>
       </c>
       <c r="J7">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K7">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -966,7 +966,7 @@
         <v>0.08</v>
       </c>
       <c r="O7">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1004,10 +1004,10 @@
         <v>16</v>
       </c>
       <c r="J8">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K8">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1019,7 +1019,7 @@
         <v>0.08</v>
       </c>
       <c r="O8">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1057,10 +1057,10 @@
         <v>16</v>
       </c>
       <c r="J9">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K9">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1072,7 +1072,7 @@
         <v>0.08</v>
       </c>
       <c r="O9">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1110,10 +1110,10 @@
         <v>16</v>
       </c>
       <c r="J10">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K10">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1125,7 +1125,7 @@
         <v>0.08</v>
       </c>
       <c r="O10">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1163,10 +1163,10 @@
         <v>16</v>
       </c>
       <c r="J11">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K11">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1178,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1216,10 +1216,10 @@
         <v>16</v>
       </c>
       <c r="J12">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K12">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1231,7 +1231,7 @@
         <v>0.08</v>
       </c>
       <c r="O12">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1269,10 +1269,10 @@
         <v>16</v>
       </c>
       <c r="J13">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K13">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1284,7 +1284,7 @@
         <v>0.08</v>
       </c>
       <c r="O13">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -1322,10 +1322,10 @@
         <v>16</v>
       </c>
       <c r="J14">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K14">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -1337,7 +1337,7 @@
         <v>0.08</v>
       </c>
       <c r="O14">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -1375,10 +1375,10 @@
         <v>16</v>
       </c>
       <c r="J15">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K15">
-        <v>5.0000000000000002E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1390,7 +1390,7 @@
         <v>0.08</v>
       </c>
       <c r="O15">
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -1428,10 +1428,10 @@
         <v>16</v>
       </c>
       <c r="J16" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K16" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L16" s="2">
         <v>0</v>
@@ -1442,8 +1442,8 @@
       <c r="N16">
         <v>0.08</v>
       </c>
-      <c r="O16">
-        <v>5.0000000000000002E-5</v>
+      <c r="O16" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P16" s="2">
         <v>0</v>
@@ -1481,10 +1481,10 @@
         <v>16</v>
       </c>
       <c r="J17" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K17" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L17" s="2">
         <v>0</v>
@@ -1495,8 +1495,8 @@
       <c r="N17">
         <v>0.08</v>
       </c>
-      <c r="O17">
-        <v>5.0000000000000002E-5</v>
+      <c r="O17" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P17" s="2">
         <v>0</v>
@@ -1534,10 +1534,10 @@
         <v>16</v>
       </c>
       <c r="J18" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K18" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L18" s="2">
         <v>0</v>
@@ -1548,8 +1548,8 @@
       <c r="N18">
         <v>0.08</v>
       </c>
-      <c r="O18">
-        <v>5.0000000000000002E-5</v>
+      <c r="O18" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P18" s="2">
         <v>0</v>
@@ -1587,10 +1587,10 @@
         <v>16</v>
       </c>
       <c r="J19" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K19" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L19" s="2">
         <v>0</v>
@@ -1601,8 +1601,8 @@
       <c r="N19">
         <v>0.08</v>
       </c>
-      <c r="O19">
-        <v>5.0000000000000002E-5</v>
+      <c r="O19" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P19" s="2">
         <v>0</v>
@@ -1640,10 +1640,10 @@
         <v>16</v>
       </c>
       <c r="J20" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K20" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L20" s="2">
         <v>0</v>
@@ -1654,8 +1654,8 @@
       <c r="N20">
         <v>0.08</v>
       </c>
-      <c r="O20">
-        <v>5.0000000000000002E-5</v>
+      <c r="O20" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P20" s="2">
         <v>0</v>
@@ -1693,10 +1693,10 @@
         <v>16</v>
       </c>
       <c r="J21" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K21" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L21" s="2">
         <v>0</v>
@@ -1707,8 +1707,8 @@
       <c r="N21">
         <v>0.08</v>
       </c>
-      <c r="O21">
-        <v>5.0000000000000002E-5</v>
+      <c r="O21" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P21" s="2">
         <v>0</v>
@@ -1746,10 +1746,10 @@
         <v>16</v>
       </c>
       <c r="J22" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K22" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L22" s="2">
         <v>0</v>
@@ -1760,8 +1760,8 @@
       <c r="N22">
         <v>0.08</v>
       </c>
-      <c r="O22">
-        <v>5.0000000000000002E-5</v>
+      <c r="O22" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P22" s="2">
         <v>0</v>
@@ -1799,10 +1799,10 @@
         <v>16</v>
       </c>
       <c r="J23" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K23" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L23" s="2">
         <v>0</v>
@@ -1813,8 +1813,8 @@
       <c r="N23">
         <v>0.08</v>
       </c>
-      <c r="O23">
-        <v>5.0000000000000002E-5</v>
+      <c r="O23" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P23" s="2">
         <v>0</v>
@@ -1852,10 +1852,10 @@
         <v>16</v>
       </c>
       <c r="J24" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K24" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L24" s="2">
         <v>0</v>
@@ -1866,8 +1866,8 @@
       <c r="N24">
         <v>0.08</v>
       </c>
-      <c r="O24">
-        <v>5.0000000000000002E-5</v>
+      <c r="O24" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P24" s="2">
         <v>0</v>
@@ -1905,10 +1905,10 @@
         <v>16</v>
       </c>
       <c r="J25" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K25" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L25" s="2">
         <v>0</v>
@@ -1919,8 +1919,8 @@
       <c r="N25">
         <v>0.08</v>
       </c>
-      <c r="O25">
-        <v>5.0000000000000002E-5</v>
+      <c r="O25" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P25" s="2">
         <v>0</v>
@@ -1958,10 +1958,10 @@
         <v>16</v>
       </c>
       <c r="J26" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K26" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L26" s="2">
         <v>0</v>
@@ -1972,8 +1972,8 @@
       <c r="N26">
         <v>0.08</v>
       </c>
-      <c r="O26">
-        <v>5.0000000000000002E-5</v>
+      <c r="O26" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P26" s="2">
         <v>0</v>
@@ -2011,10 +2011,10 @@
         <v>16</v>
       </c>
       <c r="J27" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K27" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L27" s="2">
         <v>0</v>
@@ -2025,8 +2025,8 @@
       <c r="N27">
         <v>0.08</v>
       </c>
-      <c r="O27">
-        <v>5.0000000000000002E-5</v>
+      <c r="O27" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P27" s="2">
         <v>0</v>
@@ -2064,10 +2064,10 @@
         <v>16</v>
       </c>
       <c r="J28" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K28" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L28" s="2">
         <v>0</v>
@@ -2078,8 +2078,8 @@
       <c r="N28">
         <v>0.08</v>
       </c>
-      <c r="O28">
-        <v>5.0000000000000002E-5</v>
+      <c r="O28" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P28" s="2">
         <v>0</v>
@@ -2117,10 +2117,10 @@
         <v>16</v>
       </c>
       <c r="J29" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K29" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L29" s="2">
         <v>0</v>
@@ -2131,8 +2131,8 @@
       <c r="N29">
         <v>0.08</v>
       </c>
-      <c r="O29">
-        <v>5.0000000000000002E-5</v>
+      <c r="O29" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P29" s="2">
         <v>0</v>
@@ -2170,10 +2170,10 @@
         <v>16</v>
       </c>
       <c r="J30" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K30" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L30" s="2">
         <v>0</v>
@@ -2184,8 +2184,8 @@
       <c r="N30">
         <v>0.08</v>
       </c>
-      <c r="O30">
-        <v>5.0000000000000002E-5</v>
+      <c r="O30" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P30" s="2">
         <v>0</v>
@@ -2223,10 +2223,10 @@
         <v>16</v>
       </c>
       <c r="J31" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K31" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L31" s="2">
         <v>0</v>
@@ -2237,8 +2237,8 @@
       <c r="N31">
         <v>0.08</v>
       </c>
-      <c r="O31">
-        <v>5.0000000000000002E-5</v>
+      <c r="O31" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P31" s="2">
         <v>0</v>
@@ -2276,10 +2276,10 @@
         <v>16</v>
       </c>
       <c r="J32" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K32" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L32" s="2">
         <v>0</v>
@@ -2290,8 +2290,8 @@
       <c r="N32">
         <v>0.08</v>
       </c>
-      <c r="O32">
-        <v>5.0000000000000002E-5</v>
+      <c r="O32" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P32" s="2">
         <v>0</v>
@@ -2329,10 +2329,10 @@
         <v>16</v>
       </c>
       <c r="J33" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K33" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L33" s="2">
         <v>0</v>
@@ -2343,8 +2343,8 @@
       <c r="N33">
         <v>0.08</v>
       </c>
-      <c r="O33">
-        <v>5.0000000000000002E-5</v>
+      <c r="O33" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P33" s="2">
         <v>0</v>
@@ -2382,10 +2382,10 @@
         <v>16</v>
       </c>
       <c r="J34" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K34" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L34" s="2">
         <v>0</v>
@@ -2396,8 +2396,8 @@
       <c r="N34">
         <v>0.08</v>
       </c>
-      <c r="O34">
-        <v>5.0000000000000002E-5</v>
+      <c r="O34" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P34" s="2">
         <v>0</v>
@@ -2435,10 +2435,10 @@
         <v>16</v>
       </c>
       <c r="J35" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K35" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L35" s="2">
         <v>0</v>
@@ -2449,8 +2449,8 @@
       <c r="N35">
         <v>0.08</v>
       </c>
-      <c r="O35">
-        <v>5.0000000000000002E-5</v>
+      <c r="O35" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P35" s="2">
         <v>0</v>
@@ -2488,10 +2488,10 @@
         <v>16</v>
       </c>
       <c r="J36" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K36" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L36" s="2">
         <v>0</v>
@@ -2502,8 +2502,8 @@
       <c r="N36">
         <v>0.08</v>
       </c>
-      <c r="O36">
-        <v>5.0000000000000002E-5</v>
+      <c r="O36" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P36" s="2">
         <v>0</v>
@@ -2541,10 +2541,10 @@
         <v>16</v>
       </c>
       <c r="J37" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K37" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L37" s="2">
         <v>0</v>
@@ -2555,8 +2555,8 @@
       <c r="N37">
         <v>0.08</v>
       </c>
-      <c r="O37">
-        <v>5.0000000000000002E-5</v>
+      <c r="O37" s="2">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="P37" s="2">
         <v>0</v>
@@ -2594,10 +2594,10 @@
         <v>16</v>
       </c>
       <c r="J38" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K38" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L38" s="2">
         <v>0</v>
@@ -2608,8 +2608,8 @@
       <c r="N38">
         <v>0.08</v>
       </c>
-      <c r="O38">
-        <v>5.0000000000000002E-5</v>
+      <c r="O38" s="2">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="P38" s="2">
         <v>0</v>
@@ -2647,10 +2647,10 @@
         <v>16</v>
       </c>
       <c r="J39" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K39" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L39" s="2">
         <v>0</v>
@@ -2661,8 +2661,8 @@
       <c r="N39">
         <v>0.08</v>
       </c>
-      <c r="O39">
-        <v>5.0000000000000002E-5</v>
+      <c r="O39" s="2">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="P39" s="2">
         <v>0</v>
@@ -2700,10 +2700,10 @@
         <v>16</v>
       </c>
       <c r="J40" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K40" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L40" s="2">
         <v>0</v>
@@ -2714,8 +2714,8 @@
       <c r="N40">
         <v>0.08</v>
       </c>
-      <c r="O40">
-        <v>5.0000000000000002E-5</v>
+      <c r="O40" s="2">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="P40" s="2">
         <v>0</v>
@@ -2753,10 +2753,10 @@
         <v>16</v>
       </c>
       <c r="J41" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K41" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L41" s="2">
         <v>0</v>
@@ -2767,8 +2767,8 @@
       <c r="N41">
         <v>0.08</v>
       </c>
-      <c r="O41">
-        <v>5.0000000000000002E-5</v>
+      <c r="O41" s="2">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="P41" s="2">
         <v>0</v>
@@ -2806,10 +2806,10 @@
         <v>16</v>
       </c>
       <c r="J42" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K42" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L42" s="2">
         <v>0</v>
@@ -2820,8 +2820,8 @@
       <c r="N42">
         <v>0.08</v>
       </c>
-      <c r="O42">
-        <v>5.0000000000000002E-5</v>
+      <c r="O42" s="2">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="P42" s="2">
         <v>0</v>
@@ -2859,10 +2859,10 @@
         <v>16</v>
       </c>
       <c r="J43" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K43" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L43" s="2">
         <v>0</v>
@@ -2873,8 +2873,8 @@
       <c r="N43">
         <v>0.08</v>
       </c>
-      <c r="O43">
-        <v>5.0000000000000002E-5</v>
+      <c r="O43" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P43" s="2">
         <v>0</v>
@@ -2912,10 +2912,10 @@
         <v>16</v>
       </c>
       <c r="J44" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K44" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L44" s="2">
         <v>0</v>
@@ -2926,8 +2926,8 @@
       <c r="N44">
         <v>0.08</v>
       </c>
-      <c r="O44">
-        <v>5.0000000000000002E-5</v>
+      <c r="O44" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P44" s="2">
         <v>0</v>
@@ -2965,10 +2965,10 @@
         <v>16</v>
       </c>
       <c r="J45" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K45" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L45" s="2">
         <v>0</v>
@@ -2979,8 +2979,8 @@
       <c r="N45">
         <v>0.08</v>
       </c>
-      <c r="O45">
-        <v>5.0000000000000002E-5</v>
+      <c r="O45" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P45" s="2">
         <v>0</v>
@@ -3018,10 +3018,10 @@
         <v>16</v>
       </c>
       <c r="J46" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K46" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L46" s="2">
         <v>0</v>
@@ -3032,8 +3032,8 @@
       <c r="N46">
         <v>0.08</v>
       </c>
-      <c r="O46">
-        <v>5.0000000000000002E-5</v>
+      <c r="O46" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P46" s="2">
         <v>0</v>
@@ -3071,10 +3071,10 @@
         <v>16</v>
       </c>
       <c r="J47" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K47" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L47" s="2">
         <v>0</v>
@@ -3085,8 +3085,8 @@
       <c r="N47">
         <v>0.08</v>
       </c>
-      <c r="O47">
-        <v>5.0000000000000002E-5</v>
+      <c r="O47" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P47" s="2">
         <v>0</v>
@@ -3124,10 +3124,10 @@
         <v>16</v>
       </c>
       <c r="J48" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K48" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L48" s="2">
         <v>0</v>
@@ -3138,8 +3138,8 @@
       <c r="N48">
         <v>0.08</v>
       </c>
-      <c r="O48">
-        <v>5.0000000000000002E-5</v>
+      <c r="O48" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P48" s="2">
         <v>0</v>
@@ -3177,10 +3177,10 @@
         <v>16</v>
       </c>
       <c r="J49" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K49" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L49" s="2">
         <v>0</v>
@@ -3191,8 +3191,8 @@
       <c r="N49">
         <v>0</v>
       </c>
-      <c r="O49">
-        <v>5.0000000000000002E-5</v>
+      <c r="O49" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P49" s="2">
         <v>0</v>
@@ -3230,10 +3230,10 @@
         <v>16</v>
       </c>
       <c r="J50" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K50" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L50" s="2">
         <v>0</v>
@@ -3244,8 +3244,8 @@
       <c r="N50">
         <v>0</v>
       </c>
-      <c r="O50">
-        <v>5.0000000000000002E-5</v>
+      <c r="O50" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P50" s="2">
         <v>0</v>
@@ -3283,10 +3283,10 @@
         <v>16</v>
       </c>
       <c r="J51" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K51" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L51" s="2">
         <v>0</v>
@@ -3297,8 +3297,8 @@
       <c r="N51">
         <v>0</v>
       </c>
-      <c r="O51">
-        <v>5.0000000000000002E-5</v>
+      <c r="O51" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P51" s="2">
         <v>0</v>
@@ -3336,10 +3336,10 @@
         <v>16</v>
       </c>
       <c r="J52" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K52" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L52" s="2">
         <v>0</v>
@@ -3350,8 +3350,8 @@
       <c r="N52">
         <v>0.08</v>
       </c>
-      <c r="O52">
-        <v>5.0000000000000002E-5</v>
+      <c r="O52" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P52" s="2">
         <v>0</v>
@@ -3389,10 +3389,10 @@
         <v>16</v>
       </c>
       <c r="J53" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K53" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L53" s="2">
         <v>0</v>
@@ -3403,8 +3403,8 @@
       <c r="N53">
         <v>0.08</v>
       </c>
-      <c r="O53">
-        <v>5.0000000000000002E-5</v>
+      <c r="O53" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P53" s="2">
         <v>0</v>
@@ -3442,10 +3442,10 @@
         <v>16</v>
       </c>
       <c r="J54" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K54" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L54" s="2">
         <v>0</v>
@@ -3456,8 +3456,8 @@
       <c r="N54">
         <v>0.08</v>
       </c>
-      <c r="O54">
-        <v>5.0000000000000002E-5</v>
+      <c r="O54" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P54" s="2">
         <v>0</v>
@@ -3495,10 +3495,10 @@
         <v>16</v>
       </c>
       <c r="J55" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K55" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L55" s="2">
         <v>0</v>
@@ -3509,8 +3509,8 @@
       <c r="N55">
         <v>0.08</v>
       </c>
-      <c r="O55">
-        <v>5.0000000000000002E-5</v>
+      <c r="O55" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P55" s="2">
         <v>0</v>
@@ -3548,10 +3548,10 @@
         <v>16</v>
       </c>
       <c r="J56" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K56" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L56" s="2">
         <v>0</v>
@@ -3562,8 +3562,8 @@
       <c r="N56">
         <v>0.08</v>
       </c>
-      <c r="O56">
-        <v>5.0000000000000002E-5</v>
+      <c r="O56" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P56" s="2">
         <v>0</v>
@@ -3601,10 +3601,10 @@
         <v>16</v>
       </c>
       <c r="J57" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K57" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L57" s="2">
         <v>0</v>
@@ -3615,8 +3615,8 @@
       <c r="N57">
         <v>0.08</v>
       </c>
-      <c r="O57">
-        <v>5.0000000000000002E-5</v>
+      <c r="O57" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P57" s="2">
         <v>0</v>
@@ -3654,10 +3654,10 @@
         <v>16</v>
       </c>
       <c r="J58" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="K58" s="2">
-        <v>3.0000000000000001E-5</v>
+        <v>2E-3</v>
       </c>
       <c r="L58" s="2">
         <v>0</v>
@@ -3668,8 +3668,8 @@
       <c r="N58">
         <v>0.08</v>
       </c>
-      <c r="O58">
-        <v>5.0000000000000002E-5</v>
+      <c r="O58" s="2">
+        <v>2E-3</v>
       </c>
       <c r="P58" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
OW-976, updated test results
</commit_message>
<xml_diff>
--- a/test/availAsset.xlsx
+++ b/test/availAsset.xlsx
@@ -593,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="B46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16:O58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,10 +686,10 @@
         <v>16</v>
       </c>
       <c r="J2">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K2">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -701,7 +701,7 @@
         <v>0.08</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -739,10 +739,10 @@
         <v>16</v>
       </c>
       <c r="J3">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K3">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -754,7 +754,7 @@
         <v>0.08</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -792,10 +792,10 @@
         <v>16</v>
       </c>
       <c r="J4">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K4">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -807,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -845,10 +845,10 @@
         <v>16</v>
       </c>
       <c r="J5">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K5">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -860,7 +860,7 @@
         <v>0.08</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -898,10 +898,10 @@
         <v>16</v>
       </c>
       <c r="J6">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K6">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -913,7 +913,7 @@
         <v>0.08</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -951,10 +951,10 @@
         <v>16</v>
       </c>
       <c r="J7">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K7">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -966,7 +966,7 @@
         <v>0.08</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1004,10 +1004,10 @@
         <v>16</v>
       </c>
       <c r="J8">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K8">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1019,7 +1019,7 @@
         <v>0.08</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P8">
         <v>0</v>
@@ -1057,10 +1057,10 @@
         <v>16</v>
       </c>
       <c r="J9">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K9">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1072,7 +1072,7 @@
         <v>0.08</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1110,10 +1110,10 @@
         <v>16</v>
       </c>
       <c r="J10">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K10">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1125,7 +1125,7 @@
         <v>0.08</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1163,10 +1163,10 @@
         <v>16</v>
       </c>
       <c r="J11">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K11">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1178,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P11">
         <v>0</v>
@@ -1216,10 +1216,10 @@
         <v>16</v>
       </c>
       <c r="J12">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K12">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -1231,7 +1231,7 @@
         <v>0.08</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1269,10 +1269,10 @@
         <v>16</v>
       </c>
       <c r="J13">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K13">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1284,7 +1284,7 @@
         <v>0.08</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -1322,10 +1322,10 @@
         <v>16</v>
       </c>
       <c r="J14">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K14">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -1337,7 +1337,7 @@
         <v>0.08</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -1375,10 +1375,10 @@
         <v>16</v>
       </c>
       <c r="J15">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K15">
-        <v>2E-3</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1390,7 +1390,7 @@
         <v>0.08</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="P15">
         <v>0</v>
@@ -1428,10 +1428,10 @@
         <v>16</v>
       </c>
       <c r="J16" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K16" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L16" s="2">
         <v>0</v>
@@ -1442,8 +1442,8 @@
       <c r="N16">
         <v>0.08</v>
       </c>
-      <c r="O16" s="2">
-        <v>2E-3</v>
+      <c r="O16">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P16" s="2">
         <v>0</v>
@@ -1481,10 +1481,10 @@
         <v>16</v>
       </c>
       <c r="J17" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K17" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L17" s="2">
         <v>0</v>
@@ -1495,8 +1495,8 @@
       <c r="N17">
         <v>0.08</v>
       </c>
-      <c r="O17" s="2">
-        <v>2E-3</v>
+      <c r="O17">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P17" s="2">
         <v>0</v>
@@ -1534,10 +1534,10 @@
         <v>16</v>
       </c>
       <c r="J18" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K18" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L18" s="2">
         <v>0</v>
@@ -1548,8 +1548,8 @@
       <c r="N18">
         <v>0.08</v>
       </c>
-      <c r="O18" s="2">
-        <v>2E-3</v>
+      <c r="O18">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P18" s="2">
         <v>0</v>
@@ -1587,10 +1587,10 @@
         <v>16</v>
       </c>
       <c r="J19" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K19" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L19" s="2">
         <v>0</v>
@@ -1601,8 +1601,8 @@
       <c r="N19">
         <v>0.08</v>
       </c>
-      <c r="O19" s="2">
-        <v>2E-3</v>
+      <c r="O19">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P19" s="2">
         <v>0</v>
@@ -1640,10 +1640,10 @@
         <v>16</v>
       </c>
       <c r="J20" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K20" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L20" s="2">
         <v>0</v>
@@ -1654,8 +1654,8 @@
       <c r="N20">
         <v>0.08</v>
       </c>
-      <c r="O20" s="2">
-        <v>2E-3</v>
+      <c r="O20">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P20" s="2">
         <v>0</v>
@@ -1693,10 +1693,10 @@
         <v>16</v>
       </c>
       <c r="J21" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K21" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L21" s="2">
         <v>0</v>
@@ -1707,8 +1707,8 @@
       <c r="N21">
         <v>0.08</v>
       </c>
-      <c r="O21" s="2">
-        <v>2E-3</v>
+      <c r="O21">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P21" s="2">
         <v>0</v>
@@ -1746,10 +1746,10 @@
         <v>16</v>
       </c>
       <c r="J22" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K22" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L22" s="2">
         <v>0</v>
@@ -1760,8 +1760,8 @@
       <c r="N22">
         <v>0.08</v>
       </c>
-      <c r="O22" s="2">
-        <v>2E-3</v>
+      <c r="O22">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P22" s="2">
         <v>0</v>
@@ -1799,10 +1799,10 @@
         <v>16</v>
       </c>
       <c r="J23" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K23" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L23" s="2">
         <v>0</v>
@@ -1813,8 +1813,8 @@
       <c r="N23">
         <v>0.08</v>
       </c>
-      <c r="O23" s="2">
-        <v>2E-3</v>
+      <c r="O23">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P23" s="2">
         <v>0</v>
@@ -1852,10 +1852,10 @@
         <v>16</v>
       </c>
       <c r="J24" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K24" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L24" s="2">
         <v>0</v>
@@ -1866,8 +1866,8 @@
       <c r="N24">
         <v>0.08</v>
       </c>
-      <c r="O24" s="2">
-        <v>2E-3</v>
+      <c r="O24">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P24" s="2">
         <v>0</v>
@@ -1905,10 +1905,10 @@
         <v>16</v>
       </c>
       <c r="J25" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K25" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L25" s="2">
         <v>0</v>
@@ -1919,8 +1919,8 @@
       <c r="N25">
         <v>0.08</v>
       </c>
-      <c r="O25" s="2">
-        <v>2E-3</v>
+      <c r="O25">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P25" s="2">
         <v>0</v>
@@ -1958,10 +1958,10 @@
         <v>16</v>
       </c>
       <c r="J26" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K26" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L26" s="2">
         <v>0</v>
@@ -1972,8 +1972,8 @@
       <c r="N26">
         <v>0.08</v>
       </c>
-      <c r="O26" s="2">
-        <v>2E-3</v>
+      <c r="O26">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P26" s="2">
         <v>0</v>
@@ -2011,10 +2011,10 @@
         <v>16</v>
       </c>
       <c r="J27" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K27" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L27" s="2">
         <v>0</v>
@@ -2025,8 +2025,8 @@
       <c r="N27">
         <v>0.08</v>
       </c>
-      <c r="O27" s="2">
-        <v>2E-3</v>
+      <c r="O27">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P27" s="2">
         <v>0</v>
@@ -2064,10 +2064,10 @@
         <v>16</v>
       </c>
       <c r="J28" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K28" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L28" s="2">
         <v>0</v>
@@ -2078,8 +2078,8 @@
       <c r="N28">
         <v>0.08</v>
       </c>
-      <c r="O28" s="2">
-        <v>2E-3</v>
+      <c r="O28">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P28" s="2">
         <v>0</v>
@@ -2117,10 +2117,10 @@
         <v>16</v>
       </c>
       <c r="J29" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K29" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L29" s="2">
         <v>0</v>
@@ -2131,8 +2131,8 @@
       <c r="N29">
         <v>0.08</v>
       </c>
-      <c r="O29" s="2">
-        <v>2E-3</v>
+      <c r="O29">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P29" s="2">
         <v>0</v>
@@ -2170,10 +2170,10 @@
         <v>16</v>
       </c>
       <c r="J30" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K30" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L30" s="2">
         <v>0</v>
@@ -2184,8 +2184,8 @@
       <c r="N30">
         <v>0.08</v>
       </c>
-      <c r="O30" s="2">
-        <v>2E-3</v>
+      <c r="O30">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P30" s="2">
         <v>0</v>
@@ -2223,10 +2223,10 @@
         <v>16</v>
       </c>
       <c r="J31" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K31" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L31" s="2">
         <v>0</v>
@@ -2237,8 +2237,8 @@
       <c r="N31">
         <v>0.08</v>
       </c>
-      <c r="O31" s="2">
-        <v>2E-3</v>
+      <c r="O31">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P31" s="2">
         <v>0</v>
@@ -2276,10 +2276,10 @@
         <v>16</v>
       </c>
       <c r="J32" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K32" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L32" s="2">
         <v>0</v>
@@ -2290,8 +2290,8 @@
       <c r="N32">
         <v>0.08</v>
       </c>
-      <c r="O32" s="2">
-        <v>2E-3</v>
+      <c r="O32">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P32" s="2">
         <v>0</v>
@@ -2329,10 +2329,10 @@
         <v>16</v>
       </c>
       <c r="J33" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K33" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L33" s="2">
         <v>0</v>
@@ -2343,8 +2343,8 @@
       <c r="N33">
         <v>0.08</v>
       </c>
-      <c r="O33" s="2">
-        <v>2E-3</v>
+      <c r="O33">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P33" s="2">
         <v>0</v>
@@ -2382,10 +2382,10 @@
         <v>16</v>
       </c>
       <c r="J34" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K34" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L34" s="2">
         <v>0</v>
@@ -2396,8 +2396,8 @@
       <c r="N34">
         <v>0.08</v>
       </c>
-      <c r="O34" s="2">
-        <v>2E-3</v>
+      <c r="O34">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P34" s="2">
         <v>0</v>
@@ -2435,10 +2435,10 @@
         <v>16</v>
       </c>
       <c r="J35" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K35" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L35" s="2">
         <v>0</v>
@@ -2449,8 +2449,8 @@
       <c r="N35">
         <v>0.08</v>
       </c>
-      <c r="O35" s="2">
-        <v>2E-3</v>
+      <c r="O35">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P35" s="2">
         <v>0</v>
@@ -2488,10 +2488,10 @@
         <v>16</v>
       </c>
       <c r="J36" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K36" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L36" s="2">
         <v>0</v>
@@ -2502,8 +2502,8 @@
       <c r="N36">
         <v>0.08</v>
       </c>
-      <c r="O36" s="2">
-        <v>2E-3</v>
+      <c r="O36">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P36" s="2">
         <v>0</v>
@@ -2541,10 +2541,10 @@
         <v>16</v>
       </c>
       <c r="J37" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K37" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L37" s="2">
         <v>0</v>
@@ -2555,8 +2555,8 @@
       <c r="N37">
         <v>0.08</v>
       </c>
-      <c r="O37" s="2">
-        <v>5.0000000000000001E-3</v>
+      <c r="O37">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P37" s="2">
         <v>0</v>
@@ -2594,10 +2594,10 @@
         <v>16</v>
       </c>
       <c r="J38" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K38" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L38" s="2">
         <v>0</v>
@@ -2608,8 +2608,8 @@
       <c r="N38">
         <v>0.08</v>
       </c>
-      <c r="O38" s="2">
-        <v>5.0000000000000001E-3</v>
+      <c r="O38">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P38" s="2">
         <v>0</v>
@@ -2647,10 +2647,10 @@
         <v>16</v>
       </c>
       <c r="J39" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K39" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L39" s="2">
         <v>0</v>
@@ -2661,8 +2661,8 @@
       <c r="N39">
         <v>0.08</v>
       </c>
-      <c r="O39" s="2">
-        <v>5.0000000000000001E-3</v>
+      <c r="O39">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P39" s="2">
         <v>0</v>
@@ -2700,10 +2700,10 @@
         <v>16</v>
       </c>
       <c r="J40" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K40" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L40" s="2">
         <v>0</v>
@@ -2714,8 +2714,8 @@
       <c r="N40">
         <v>0.08</v>
       </c>
-      <c r="O40" s="2">
-        <v>5.0000000000000001E-3</v>
+      <c r="O40">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P40" s="2">
         <v>0</v>
@@ -2753,10 +2753,10 @@
         <v>16</v>
       </c>
       <c r="J41" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K41" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L41" s="2">
         <v>0</v>
@@ -2767,8 +2767,8 @@
       <c r="N41">
         <v>0.08</v>
       </c>
-      <c r="O41" s="2">
-        <v>5.0000000000000001E-3</v>
+      <c r="O41">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P41" s="2">
         <v>0</v>
@@ -2806,10 +2806,10 @@
         <v>16</v>
       </c>
       <c r="J42" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K42" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L42" s="2">
         <v>0</v>
@@ -2820,8 +2820,8 @@
       <c r="N42">
         <v>0.08</v>
       </c>
-      <c r="O42" s="2">
-        <v>5.0000000000000001E-3</v>
+      <c r="O42">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P42" s="2">
         <v>0</v>
@@ -2859,10 +2859,10 @@
         <v>16</v>
       </c>
       <c r="J43" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K43" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L43" s="2">
         <v>0</v>
@@ -2873,8 +2873,8 @@
       <c r="N43">
         <v>0.08</v>
       </c>
-      <c r="O43" s="2">
-        <v>2E-3</v>
+      <c r="O43">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P43" s="2">
         <v>0</v>
@@ -2912,10 +2912,10 @@
         <v>16</v>
       </c>
       <c r="J44" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K44" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L44" s="2">
         <v>0</v>
@@ -2926,8 +2926,8 @@
       <c r="N44">
         <v>0.08</v>
       </c>
-      <c r="O44" s="2">
-        <v>2E-3</v>
+      <c r="O44">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P44" s="2">
         <v>0</v>
@@ -2965,10 +2965,10 @@
         <v>16</v>
       </c>
       <c r="J45" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K45" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L45" s="2">
         <v>0</v>
@@ -2979,8 +2979,8 @@
       <c r="N45">
         <v>0.08</v>
       </c>
-      <c r="O45" s="2">
-        <v>2E-3</v>
+      <c r="O45">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P45" s="2">
         <v>0</v>
@@ -3018,10 +3018,10 @@
         <v>16</v>
       </c>
       <c r="J46" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K46" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L46" s="2">
         <v>0</v>
@@ -3032,8 +3032,8 @@
       <c r="N46">
         <v>0.08</v>
       </c>
-      <c r="O46" s="2">
-        <v>2E-3</v>
+      <c r="O46">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P46" s="2">
         <v>0</v>
@@ -3071,10 +3071,10 @@
         <v>16</v>
       </c>
       <c r="J47" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K47" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L47" s="2">
         <v>0</v>
@@ -3085,8 +3085,8 @@
       <c r="N47">
         <v>0.08</v>
       </c>
-      <c r="O47" s="2">
-        <v>2E-3</v>
+      <c r="O47">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P47" s="2">
         <v>0</v>
@@ -3124,10 +3124,10 @@
         <v>16</v>
       </c>
       <c r="J48" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K48" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L48" s="2">
         <v>0</v>
@@ -3138,8 +3138,8 @@
       <c r="N48">
         <v>0.08</v>
       </c>
-      <c r="O48" s="2">
-        <v>2E-3</v>
+      <c r="O48">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P48" s="2">
         <v>0</v>
@@ -3177,10 +3177,10 @@
         <v>16</v>
       </c>
       <c r="J49" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K49" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L49" s="2">
         <v>0</v>
@@ -3191,8 +3191,8 @@
       <c r="N49">
         <v>0</v>
       </c>
-      <c r="O49" s="2">
-        <v>2E-3</v>
+      <c r="O49">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P49" s="2">
         <v>0</v>
@@ -3230,10 +3230,10 @@
         <v>16</v>
       </c>
       <c r="J50" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K50" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L50" s="2">
         <v>0</v>
@@ -3244,8 +3244,8 @@
       <c r="N50">
         <v>0</v>
       </c>
-      <c r="O50" s="2">
-        <v>2E-3</v>
+      <c r="O50">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P50" s="2">
         <v>0</v>
@@ -3283,10 +3283,10 @@
         <v>16</v>
       </c>
       <c r="J51" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K51" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L51" s="2">
         <v>0</v>
@@ -3297,8 +3297,8 @@
       <c r="N51">
         <v>0</v>
       </c>
-      <c r="O51" s="2">
-        <v>2E-3</v>
+      <c r="O51">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P51" s="2">
         <v>0</v>
@@ -3336,10 +3336,10 @@
         <v>16</v>
       </c>
       <c r="J52" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K52" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L52" s="2">
         <v>0</v>
@@ -3350,8 +3350,8 @@
       <c r="N52">
         <v>0.08</v>
       </c>
-      <c r="O52" s="2">
-        <v>2E-3</v>
+      <c r="O52">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P52" s="2">
         <v>0</v>
@@ -3389,10 +3389,10 @@
         <v>16</v>
       </c>
       <c r="J53" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K53" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L53" s="2">
         <v>0</v>
@@ -3403,8 +3403,8 @@
       <c r="N53">
         <v>0.08</v>
       </c>
-      <c r="O53" s="2">
-        <v>2E-3</v>
+      <c r="O53">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P53" s="2">
         <v>0</v>
@@ -3442,10 +3442,10 @@
         <v>16</v>
       </c>
       <c r="J54" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K54" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L54" s="2">
         <v>0</v>
@@ -3456,8 +3456,8 @@
       <c r="N54">
         <v>0.08</v>
       </c>
-      <c r="O54" s="2">
-        <v>2E-3</v>
+      <c r="O54">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P54" s="2">
         <v>0</v>
@@ -3495,10 +3495,10 @@
         <v>16</v>
       </c>
       <c r="J55" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K55" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L55" s="2">
         <v>0</v>
@@ -3509,8 +3509,8 @@
       <c r="N55">
         <v>0.08</v>
       </c>
-      <c r="O55" s="2">
-        <v>2E-3</v>
+      <c r="O55">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P55" s="2">
         <v>0</v>
@@ -3548,10 +3548,10 @@
         <v>16</v>
       </c>
       <c r="J56" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K56" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L56" s="2">
         <v>0</v>
@@ -3562,8 +3562,8 @@
       <c r="N56">
         <v>0.08</v>
       </c>
-      <c r="O56" s="2">
-        <v>2E-3</v>
+      <c r="O56">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P56" s="2">
         <v>0</v>
@@ -3601,10 +3601,10 @@
         <v>16</v>
       </c>
       <c r="J57" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K57" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L57" s="2">
         <v>0</v>
@@ -3615,8 +3615,8 @@
       <c r="N57">
         <v>0.08</v>
       </c>
-      <c r="O57" s="2">
-        <v>2E-3</v>
+      <c r="O57">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P57" s="2">
         <v>0</v>
@@ -3654,10 +3654,10 @@
         <v>16</v>
       </c>
       <c r="J58" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="K58" s="2">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="L58" s="2">
         <v>0</v>
@@ -3668,8 +3668,8 @@
       <c r="N58">
         <v>0.08</v>
       </c>
-      <c r="O58" s="2">
-        <v>2E-3</v>
+      <c r="O58">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="P58" s="2">
         <v>0</v>

</xml_diff>